<commit_message>
Proyecto 1 - Presupuesto
</commit_message>
<xml_diff>
--- a/Practica 1/201520498/Prueba.xlsx
+++ b/Practica 1/201520498/Prueba.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matal\OneDrive\Escritorio\Universidad\IA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LABS\IA\Lab\Lab_IA\Practica 1\201520498\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2178E20-E2C0-4C87-BC03-FF856DBAA0F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2620168B-846F-468B-A3FA-04D4869A966B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -33,10 +33,10 @@
     <t>Nacimiento</t>
   </si>
   <si>
-    <t>3191030210501</t>
+    <t xml:space="preserve">3306466721202	</t>
   </si>
   <si>
-    <t>27/08/1997</t>
+    <t>18/09/1997</t>
   </si>
 </sst>
 </file>
@@ -371,7 +371,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -398,5 +398,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>